<commit_message>
Added UI comfort changes and made fixed issue with order entry. Seems to be resolved
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/LUSARD.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/LUSARD.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,19 @@
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25 lb pasta fusi for ravioli</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>25 01TRAV</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added found customer info but no excel. Cleaned up already entered auto select stuff
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/LUSARD.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/LUSARD.xlsx
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>customer_id</t>
+          <t>cust_id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>display_name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -468,7 +468,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1 29CAVA</t>
+          <t>5 29CAVA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>

</xml_diff>